<commit_message>
Prob 1 sim works, but is slow.
</commit_message>
<xml_diff>
--- a/data_challenge/311_complaint freq table.xlsx
+++ b/data_challenge/311_complaint freq table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>agency</t>
   </si>
@@ -94,12 +94,21 @@
   </si>
   <si>
     <t>TLC</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>NYPD proportion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -142,22 +151,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,13 +501,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -698,6 +716,24 @@
       </c>
       <c r="C26">
         <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <f>SUM(C2:C26)</f>
+        <v>114349</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2">
+        <f>C3/C29</f>
+        <v>0.18979615038172612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>